<commit_message>
feat: Implement expense management features with AddExpenseForm, ExpenseList, and ExpensePageOverview components; enhance UI and functionality
</commit_message>
<xml_diff>
--- a/Backend/Expenses_details.xlsx
+++ b/Backend/Expenses_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,13 +415,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Food</v>
+        <v>Books</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-07-20</v>
+        <v>2025-07-30</v>
       </c>
     </row>
     <row r="3">
@@ -429,26 +429,81 @@
         <v>Transport</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-07-19</v>
+        <v>2025-07-29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Health</v>
+        <v>Food</v>
       </c>
       <c r="B4">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="C4" t="str">
-        <v>2025-07-19</v>
+        <v>2025-07-27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Transport</v>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-07-25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="B6">
+        <v>450</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-07-20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-07-10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>IceCream</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-07-06</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ElectricityBill</v>
+      </c>
+      <c r="B9">
+        <v>500</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-07-06</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>